<commit_message>
understand how to store and return multiple values using pojo class in reurn data class
</commit_message>
<xml_diff>
--- a/ExcelFils/verficationNew.xlsx
+++ b/ExcelFils/verficationNew.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13995" windowHeight="3285" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12285" windowHeight="2190" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="data1" sheetId="4" r:id="rId4"/>
+    <sheet name="Dynamic" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N9"/>
+  <oleSize ref="A1:L5"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>RollNo</t>
   </si>
@@ -31,6 +32,9 @@
   <si>
     <t>Vivek</t>
   </si>
+  <si>
+    <t>Sumit</t>
+  </si>
 </sst>
 </file>
 
@@ -45,12 +49,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -75,10 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -445,4 +456,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>